<commit_message>
Reworked Treasury upload to use the Projects database
</commit_message>
<xml_diff>
--- a/doc/specifications-from-treasury/Data Upload Service DataDictionary 11302020.xlsx
+++ b/doc/specifications-from-treasury/Data Upload Service DataDictionary 11302020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/usdr/cares-reporter/doc/specifications-from-treasury/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4B298D-80F9-314B-969A-5D686AD4AFBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7F2C5C-8086-6B43-B555-833E36D6CBE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="47620" windowHeight="21120" tabRatio="531" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21120" tabRatio="531" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using Toolkit" sheetId="1" state="hidden" r:id="rId1"/>
@@ -15577,7 +15577,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:B1"/>
       <selection pane="topRight" sqref="A1:B1"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
@@ -16079,12 +16079,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52FDFC9-981B-4124-8AC9-EFBF6FA5B6F3}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:B1"/>
       <selection pane="topRight" sqref="A1:B1"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
-      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -16501,8 +16501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA46BC8-0A44-497F-AEC5-3554A215BFB3}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:B1"/>
       <selection pane="topRight" sqref="A1:B1"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
@@ -16697,7 +16697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA1FD52-AA54-4F4A-A62F-78B4CD847C3A}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:B1"/>
       <selection pane="topRight" sqref="A1:B1"/>
@@ -57743,7 +57743,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:B1"/>
       <selection pane="topRight" sqref="A1:B1"/>
@@ -59893,7 +59893,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:B1"/>
       <selection pane="topRight" sqref="A1:B1"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>

</xml_diff>

<commit_message>
API and tests for reporting periods for documents
</commit_message>
<xml_diff>
--- a/doc/specifications-from-treasury/Data Upload Service DataDictionary 11302020.xlsx
+++ b/doc/specifications-from-treasury/Data Upload Service DataDictionary 11302020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/usdr/cares-reporter/doc/specifications-from-treasury/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7F2C5C-8086-6B43-B555-833E36D6CBE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1839A612-8E94-6441-8D2D-41255058950C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21120" tabRatio="531" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21120" tabRatio="531" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using Toolkit" sheetId="1" state="hidden" r:id="rId1"/>
@@ -67,8 +67,8 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Northrop Grumman User - Personal View" guid="{FC90CCDA-51EA-493F-B2B6-53D4A7BF04D4}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="605" activeSheetId="5"/>
     <customWorkbookView name="Melissa Bright Lemmond - Personal View" guid="{BBEDD245-5499-4FA4-B816-936248AFC354}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="581" activeSheetId="3"/>
-    <customWorkbookView name="Northrop Grumman User - Personal View" guid="{FC90CCDA-51EA-493F-B2B6-53D4A7BF04D4}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="605" activeSheetId="5"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -10724,6 +10724,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -10745,54 +10748,6 @@
     <xf numFmtId="0" fontId="44" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="36" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -10804,6 +10759,54 @@
     </xf>
     <xf numFmtId="0" fontId="44" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="36" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -10821,9 +10824,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="42" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -15363,20 +15363,20 @@
       <c r="A3" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="254" t="s">
+      <c r="B3" s="255" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="254"/>
+      <c r="C3" s="255"/>
     </row>
     <row r="4" spans="1:9" ht="12.75" customHeight="1" thickTop="1" thickBot="1"/>
     <row r="5" spans="1:9" ht="29.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="254" t="s">
+      <c r="B5" s="255" t="s">
         <v>215</v>
       </c>
-      <c r="C5" s="254"/>
+      <c r="C5" s="255"/>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="57"/>
@@ -15387,10 +15387,10 @@
       <c r="A7" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="254" t="s">
+      <c r="B7" s="255" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="254"/>
+      <c r="C7" s="255"/>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="57"/>
@@ -15401,10 +15401,10 @@
       <c r="A9" s="57" t="s">
         <v>217</v>
       </c>
-      <c r="B9" s="254" t="s">
+      <c r="B9" s="255" t="s">
         <v>410</v>
       </c>
-      <c r="C9" s="254"/>
+      <c r="C9" s="255"/>
     </row>
     <row r="10" spans="1:9" thickTop="1" thickBot="1">
       <c r="A10" s="61"/>
@@ -15415,10 +15415,10 @@
       <c r="A11" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="257" t="s">
+      <c r="B11" s="258" t="s">
         <v>411</v>
       </c>
-      <c r="C11" s="257"/>
+      <c r="C11" s="258"/>
     </row>
     <row r="12" spans="1:9" thickTop="1" thickBot="1">
       <c r="A12" s="61"/>
@@ -15501,10 +15501,10 @@
     </row>
     <row r="25" spans="1:3" ht="40.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A25" s="61"/>
-      <c r="B25" s="255" t="s">
+      <c r="B25" s="256" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="256"/>
+      <c r="C25" s="257"/>
     </row>
     <row r="26" spans="1:3" thickTop="1" thickBot="1">
       <c r="A26" s="61"/>
@@ -15544,13 +15544,13 @@
   </sheetData>
   <sheetProtection password="CC64" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{BBEDD245-5499-4FA4-B816-936248AFC354}" showRuler="0">
+    <customSheetView guid="{FC90CCDA-51EA-493F-B2B6-53D4A7BF04D4}" showPageBreaks="1" printArea="1" showRuler="0">
       <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
       <pageSetup scale="65" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{FC90CCDA-51EA-493F-B2B6-53D4A7BF04D4}" showPageBreaks="1" printArea="1" showRuler="0">
+    <customSheetView guid="{BBEDD245-5499-4FA4-B816-936248AFC354}" showRuler="0">
       <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
       <pageSetup scale="65" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -15857,7 +15857,7 @@
       <c r="H9" s="246" t="s">
         <v>2173</v>
       </c>
-      <c r="I9" s="287" t="s">
+      <c r="I9" s="254" t="s">
         <v>2084</v>
       </c>
       <c r="K9" s="222"/>
@@ -16697,7 +16697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA1FD52-AA54-4F4A-A62F-78B4CD847C3A}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection sqref="A1:B1"/>
       <selection pane="topRight" sqref="A1:B1"/>
@@ -28715,12 +28715,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23">
-      <c r="A1" s="271" t="s">
+      <c r="A1" s="272" t="s">
         <v>316</v>
       </c>
-      <c r="B1" s="271"/>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
+      <c r="B1" s="272"/>
+      <c r="C1" s="272"/>
+      <c r="D1" s="272"/>
     </row>
     <row r="2" spans="1:5" ht="6" customHeight="1">
       <c r="A2" s="119"/>
@@ -28729,12 +28729,12 @@
       <c r="D2" s="120"/>
     </row>
     <row r="3" spans="1:5" ht="24" customHeight="1">
-      <c r="A3" s="275" t="s">
+      <c r="A3" s="279" t="s">
         <v>348</v>
       </c>
-      <c r="B3" s="276"/>
-      <c r="C3" s="276"/>
-      <c r="D3" s="276"/>
+      <c r="B3" s="280"/>
+      <c r="C3" s="280"/>
+      <c r="D3" s="280"/>
     </row>
     <row r="4" spans="1:5" ht="14" thickBot="1">
       <c r="A4" s="121"/>
@@ -28743,14 +28743,14 @@
       <c r="D4" s="123"/>
     </row>
     <row r="5" spans="1:5" ht="14" thickTop="1">
-      <c r="A5" s="263" t="s">
+      <c r="A5" s="275" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="272"/>
-      <c r="C5" s="263" t="s">
+      <c r="B5" s="276"/>
+      <c r="C5" s="275" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="264"/>
+      <c r="D5" s="281"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5">
@@ -28760,10 +28760,10 @@
       <c r="B6" s="96" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="265" t="s">
+      <c r="C6" s="277" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="266"/>
+      <c r="D6" s="278"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5">
@@ -28773,10 +28773,10 @@
       <c r="B7" s="96" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="265" t="s">
+      <c r="C7" s="277" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="266"/>
+      <c r="D7" s="278"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5">
@@ -28786,10 +28786,10 @@
       <c r="B8" s="96" t="s">
         <v>170</v>
       </c>
-      <c r="C8" s="265" t="s">
+      <c r="C8" s="277" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="266"/>
+      <c r="D8" s="278"/>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5">
@@ -28799,10 +28799,10 @@
       <c r="B9" s="96" t="s">
         <v>169</v>
       </c>
-      <c r="C9" s="273" t="s">
+      <c r="C9" s="266" t="s">
         <v>140</v>
       </c>
-      <c r="D9" s="274"/>
+      <c r="D9" s="267"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5">
@@ -28812,10 +28812,10 @@
       <c r="B10" s="96" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="273" t="s">
+      <c r="C10" s="266" t="s">
         <v>142</v>
       </c>
-      <c r="D10" s="274"/>
+      <c r="D10" s="267"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
@@ -28825,10 +28825,10 @@
       <c r="B11" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="273" t="s">
+      <c r="C11" s="266" t="s">
         <v>185</v>
       </c>
-      <c r="D11" s="274"/>
+      <c r="D11" s="267"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="14" thickBot="1">
@@ -28838,10 +28838,10 @@
       <c r="B12" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="269" t="s">
+      <c r="C12" s="268" t="s">
         <v>308</v>
       </c>
-      <c r="D12" s="270"/>
+      <c r="D12" s="269"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="15" thickTop="1">
@@ -28866,10 +28866,10 @@
       <c r="B14" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="269" t="s">
+      <c r="C14" s="268" t="s">
         <v>309</v>
       </c>
-      <c r="D14" s="270"/>
+      <c r="D14" s="269"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="15" thickTop="1">
@@ -28901,10 +28901,10 @@
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="15" thickTop="1">
-      <c r="A17" s="279" t="s">
+      <c r="A17" s="264" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="280"/>
+      <c r="B17" s="265"/>
       <c r="C17" s="110" t="s">
         <v>319</v>
       </c>
@@ -28920,10 +28920,10 @@
       <c r="B18" s="90" t="s">
         <v>264</v>
       </c>
-      <c r="C18" s="265" t="s">
+      <c r="C18" s="277" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="266"/>
+      <c r="D18" s="278"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
@@ -28933,10 +28933,10 @@
       <c r="B19" s="90" t="s">
         <v>265</v>
       </c>
-      <c r="C19" s="265" t="s">
+      <c r="C19" s="277" t="s">
         <v>347</v>
       </c>
-      <c r="D19" s="266"/>
+      <c r="D19" s="278"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
@@ -28946,10 +28946,10 @@
       <c r="B20" s="90" t="s">
         <v>136</v>
       </c>
-      <c r="C20" s="267" t="s">
+      <c r="C20" s="273" t="s">
         <v>346</v>
       </c>
-      <c r="D20" s="268"/>
+      <c r="D20" s="274"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="14" thickBot="1">
@@ -28957,17 +28957,17 @@
       <c r="B21" s="90" t="s">
         <v>138</v>
       </c>
-      <c r="C21" s="261" t="s">
+      <c r="C21" s="270" t="s">
         <v>345</v>
       </c>
-      <c r="D21" s="262"/>
+      <c r="D21" s="271"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="15" thickTop="1">
-      <c r="A22" s="279" t="s">
+      <c r="A22" s="264" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="280"/>
+      <c r="B22" s="265"/>
       <c r="C22" s="108" t="s">
         <v>306</v>
       </c>
@@ -29005,21 +29005,21 @@
         <v>190</v>
       </c>
       <c r="B25" s="104"/>
-      <c r="C25" s="267" t="s">
+      <c r="C25" s="273" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="268"/>
+      <c r="D25" s="274"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" ht="14" thickBot="1">
-      <c r="A26" s="277" t="s">
+      <c r="A26" s="262" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="278"/>
-      <c r="C26" s="261" t="s">
+      <c r="B26" s="263"/>
+      <c r="C26" s="270" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="262"/>
+      <c r="D26" s="271"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" ht="15" thickTop="1">
@@ -29044,10 +29044,10 @@
       <c r="B28" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="261" t="s">
+      <c r="C28" s="270" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="262"/>
+      <c r="D28" s="271"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="15" thickTop="1">
@@ -29088,13 +29088,13 @@
   </sheetData>
   <sheetProtection password="CDA4" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{BBEDD245-5499-4FA4-B816-936248AFC354}" fitToPage="1" showRuler="0">
+    <customSheetView guid="{FC90CCDA-51EA-493F-B2B6-53D4A7BF04D4}" fitToPage="1" showRuler="0">
       <selection activeCell="A18" sqref="A18"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup scale="89" orientation="landscape" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{FC90CCDA-51EA-493F-B2B6-53D4A7BF04D4}" fitToPage="1" showRuler="0">
+    <customSheetView guid="{BBEDD245-5499-4FA4-B816-936248AFC354}" fitToPage="1" showRuler="0">
       <selection activeCell="A18" sqref="A18"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup scale="89" orientation="landscape" r:id="rId2"/>
@@ -29102,12 +29102,13 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="22">
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="A5:B5"/>
@@ -29117,13 +29118,12 @@
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C26:D26"/>
   </mergeCells>
   <phoneticPr fontId="34" type="noConversion"/>
   <hyperlinks>
@@ -29268,16 +29268,16 @@
       <c r="Q2" s="48"/>
     </row>
     <row r="3" spans="1:17" s="11" customFormat="1" ht="62.25" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A3" s="283" t="s">
+      <c r="A3" s="284" t="s">
         <v>218</v>
       </c>
-      <c r="B3" s="284"/>
-      <c r="C3" s="284"/>
-      <c r="D3" s="284"/>
-      <c r="E3" s="284"/>
-      <c r="F3" s="284"/>
-      <c r="G3" s="284"/>
-      <c r="H3" s="285"/>
+      <c r="B3" s="285"/>
+      <c r="C3" s="285"/>
+      <c r="D3" s="285"/>
+      <c r="E3" s="285"/>
+      <c r="F3" s="285"/>
+      <c r="G3" s="285"/>
+      <c r="H3" s="286"/>
       <c r="I3" s="51"/>
       <c r="J3" s="50"/>
       <c r="K3" s="50"/>
@@ -29433,25 +29433,25 @@
       <c r="Q7" s="17"/>
     </row>
     <row r="8" spans="1:17" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A8" s="281" t="s">
+      <c r="A8" s="282" t="s">
         <v>288</v>
       </c>
-      <c r="B8" s="281"/>
-      <c r="C8" s="281"/>
-      <c r="D8" s="281"/>
-      <c r="E8" s="281"/>
-      <c r="F8" s="281"/>
-      <c r="G8" s="281"/>
-      <c r="H8" s="281"/>
-      <c r="I8" s="281"/>
-      <c r="J8" s="281"/>
-      <c r="K8" s="281"/>
-      <c r="L8" s="281"/>
-      <c r="M8" s="281"/>
-      <c r="N8" s="281"/>
-      <c r="O8" s="281"/>
-      <c r="P8" s="281"/>
-      <c r="Q8" s="282"/>
+      <c r="B8" s="282"/>
+      <c r="C8" s="282"/>
+      <c r="D8" s="282"/>
+      <c r="E8" s="282"/>
+      <c r="F8" s="282"/>
+      <c r="G8" s="282"/>
+      <c r="H8" s="282"/>
+      <c r="I8" s="282"/>
+      <c r="J8" s="282"/>
+      <c r="K8" s="282"/>
+      <c r="L8" s="282"/>
+      <c r="M8" s="282"/>
+      <c r="N8" s="282"/>
+      <c r="O8" s="282"/>
+      <c r="P8" s="282"/>
+      <c r="Q8" s="283"/>
     </row>
     <row r="9" spans="1:17" s="12" customFormat="1" ht="25.5" customHeight="1">
       <c r="A9" s="71" t="s">
@@ -31289,25 +31289,25 @@
       <c r="Q47" s="76"/>
     </row>
     <row r="48" spans="1:17" s="15" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A48" s="286" t="s">
+      <c r="A48" s="287" t="s">
         <v>172</v>
       </c>
-      <c r="B48" s="286"/>
-      <c r="C48" s="286"/>
-      <c r="D48" s="286"/>
-      <c r="E48" s="286"/>
-      <c r="F48" s="286"/>
-      <c r="G48" s="286"/>
-      <c r="H48" s="286"/>
-      <c r="I48" s="286"/>
-      <c r="J48" s="286"/>
-      <c r="K48" s="286"/>
-      <c r="L48" s="286"/>
-      <c r="M48" s="286"/>
-      <c r="N48" s="286"/>
-      <c r="O48" s="286"/>
-      <c r="P48" s="286"/>
-      <c r="Q48" s="286"/>
+      <c r="B48" s="287"/>
+      <c r="C48" s="287"/>
+      <c r="D48" s="287"/>
+      <c r="E48" s="287"/>
+      <c r="F48" s="287"/>
+      <c r="G48" s="287"/>
+      <c r="H48" s="287"/>
+      <c r="I48" s="287"/>
+      <c r="J48" s="287"/>
+      <c r="K48" s="287"/>
+      <c r="L48" s="287"/>
+      <c r="M48" s="287"/>
+      <c r="N48" s="287"/>
+      <c r="O48" s="287"/>
+      <c r="P48" s="287"/>
+      <c r="Q48" s="287"/>
     </row>
     <row r="49" spans="1:17" s="14" customFormat="1" ht="26">
       <c r="A49" s="71" t="s">
@@ -31806,25 +31806,25 @@
       <c r="Q58" s="78"/>
     </row>
     <row r="59" spans="1:17" s="2" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A59" s="286" t="s">
+      <c r="A59" s="287" t="s">
         <v>171</v>
       </c>
-      <c r="B59" s="286"/>
-      <c r="C59" s="286"/>
-      <c r="D59" s="286"/>
-      <c r="E59" s="286"/>
-      <c r="F59" s="286"/>
-      <c r="G59" s="286"/>
-      <c r="H59" s="286"/>
-      <c r="I59" s="286"/>
-      <c r="J59" s="286"/>
-      <c r="K59" s="286"/>
-      <c r="L59" s="286"/>
-      <c r="M59" s="286"/>
-      <c r="N59" s="286"/>
-      <c r="O59" s="286"/>
-      <c r="P59" s="286"/>
-      <c r="Q59" s="286"/>
+      <c r="B59" s="287"/>
+      <c r="C59" s="287"/>
+      <c r="D59" s="287"/>
+      <c r="E59" s="287"/>
+      <c r="F59" s="287"/>
+      <c r="G59" s="287"/>
+      <c r="H59" s="287"/>
+      <c r="I59" s="287"/>
+      <c r="J59" s="287"/>
+      <c r="K59" s="287"/>
+      <c r="L59" s="287"/>
+      <c r="M59" s="287"/>
+      <c r="N59" s="287"/>
+      <c r="O59" s="287"/>
+      <c r="P59" s="287"/>
+      <c r="Q59" s="287"/>
     </row>
     <row r="60" spans="1:17" s="14" customFormat="1" ht="26">
       <c r="A60" s="71" t="s">
@@ -34865,7 +34865,7 @@
   </sheetData>
   <sheetProtection password="CC64" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{BBEDD245-5499-4FA4-B816-936248AFC354}" fitToPage="1" showRuler="0" topLeftCell="L1">
+    <customSheetView guid="{FC90CCDA-51EA-493F-B2B6-53D4A7BF04D4}" fitToPage="1" showRuler="0" topLeftCell="L1">
       <pane ySplit="6" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q34" sqref="Q34"/>
       <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.75" header="0.5" footer="0.5"/>
@@ -34874,7 +34874,7 @@
         <oddFooter>&amp;R&amp;P</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{FC90CCDA-51EA-493F-B2B6-53D4A7BF04D4}" fitToPage="1" showRuler="0" topLeftCell="L1">
+    <customSheetView guid="{BBEDD245-5499-4FA4-B816-936248AFC354}" fitToPage="1" showRuler="0" topLeftCell="L1">
       <pane ySplit="6" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q34" sqref="Q34"/>
       <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.75" header="0.5" footer="0.5"/>
@@ -57159,7 +57159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C524FCC1-3CAF-48F0-A440-E700F799A0E0}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -57248,10 +57248,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="258" t="s">
+      <c r="A1" s="259" t="s">
         <v>2062</v>
       </c>
-      <c r="B1" s="259"/>
+      <c r="B1" s="260"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="215" t="s">
@@ -57335,10 +57335,10 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="260" t="s">
+      <c r="A13" s="261" t="s">
         <v>2063</v>
       </c>
-      <c r="B13" s="260"/>
+      <c r="B13" s="261"/>
     </row>
     <row r="14" spans="1:3" ht="80">
       <c r="A14" s="209" t="s">
@@ -60792,18 +60792,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -60826,14 +60826,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D06BD80-EBE2-48CB-B5E7-4271B4D6D6A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC78748C-17B0-430B-8E6D-B9BAFC416B40}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="5ed1b53d-38e3-4f5b-a041-d8cba0693c5a"/>
@@ -60848,4 +60840,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D06BD80-EBE2-48CB-B5E7-4271B4D6D6A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>